<commit_message>
Add load data from excel
</commit_message>
<xml_diff>
--- a/src/main/resources/mainProtocol.xlsx
+++ b/src/main/resources/mainProtocol.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Artem\IdeaProjects\KRobotUtils\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artem_admin\IdeaProjects\KRobotUtils\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5811353-84DD-4460-B8E1-F86CDE714087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5622A737-0920-44B5-B29D-3966519766F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="10050" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -427,16 +427,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -536,8 +536,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7965915" y="8229824"/>
-          <a:ext cx="2129794" cy="827269"/>
+          <a:off x="8113919" y="8256201"/>
+          <a:ext cx="2179617" cy="823117"/>
           <a:chOff x="21" y="992"/>
           <a:chExt cx="214" cy="95"/>
         </a:xfrm>
@@ -987,8 +987,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1219283" y="8306024"/>
-          <a:ext cx="2167895" cy="827269"/>
+          <a:off x="1222214" y="8332401"/>
+          <a:ext cx="2208925" cy="823117"/>
           <a:chOff x="21" y="992"/>
           <a:chExt cx="214" cy="95"/>
         </a:xfrm>
@@ -1686,36 +1686,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:W42"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="130" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A15" zoomScale="130" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.7265625" customWidth="1"/>
-    <col min="2" max="2" width="13.26953125" customWidth="1"/>
-    <col min="5" max="5" width="4.7265625" customWidth="1"/>
-    <col min="10" max="10" width="1.54296875" customWidth="1"/>
-    <col min="12" max="12" width="8.54296875" customWidth="1"/>
-    <col min="13" max="13" width="4.54296875" customWidth="1"/>
-    <col min="14" max="14" width="13.453125" customWidth="1"/>
+    <col min="1" max="1" width="3.77734375" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" customWidth="1"/>
+    <col min="5" max="5" width="4.77734375" customWidth="1"/>
+    <col min="10" max="10" width="1.5546875" customWidth="1"/>
+    <col min="12" max="12" width="8.5546875" customWidth="1"/>
+    <col min="13" max="13" width="4.5546875" customWidth="1"/>
+    <col min="14" max="14" width="13.44140625" customWidth="1"/>
     <col min="17" max="17" width="4" customWidth="1"/>
-    <col min="22" max="22" width="1.453125" customWidth="1"/>
-    <col min="23" max="23" width="7.453125" customWidth="1"/>
-    <col min="24" max="24" width="8.7265625" customWidth="1"/>
+    <col min="22" max="22" width="1.44140625" customWidth="1"/>
+    <col min="23" max="23" width="7.44140625" customWidth="1"/>
+    <col min="24" max="24" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:23" ht="20" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:23" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="F3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:23" ht="20" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:23" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="F4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:23" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:23" ht="21" thickBot="1" x14ac:dyDescent="0.4">
       <c r="F5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1726,7 +1726,7 @@
       <c r="V5" s="11"/>
       <c r="W5" s="11"/>
     </row>
-    <row r="6" spans="2:23" ht="20.5" thickTop="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:23" ht="21" thickTop="1" x14ac:dyDescent="0.35">
       <c r="F6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1743,11 +1743,11 @@
       <c r="T6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="U6" s="25"/>
-      <c r="V6" s="25"/>
-      <c r="W6" s="26"/>
-    </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="U6" s="27"/>
+      <c r="V6" s="27"/>
+      <c r="W6" s="28"/>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.3">
       <c r="N7" s="22" t="s">
         <v>17</v>
       </c>
@@ -1765,7 +1765,7 @@
       <c r="V7" s="23"/>
       <c r="W7" s="24"/>
     </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:23" x14ac:dyDescent="0.3">
       <c r="N8" s="16"/>
       <c r="O8" s="8"/>
       <c r="P8" s="8"/>
@@ -1779,17 +1779,15 @@
       <c r="V8" s="23"/>
       <c r="W8" s="24"/>
     </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="5">
-        <v>2</v>
-      </c>
-      <c r="G9" s="27" t="s">
+      <c r="D9" s="5"/>
+      <c r="G9" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="27"/>
+      <c r="H9" s="25"/>
       <c r="I9" s="2"/>
       <c r="J9" s="3" t="s">
         <v>10</v>
@@ -1808,7 +1806,7 @@
       <c r="V9" s="8"/>
       <c r="W9" s="17"/>
     </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C10" s="6"/>
       <c r="N10" s="16"/>
       <c r="O10" s="10" t="s">
@@ -1827,21 +1825,17 @@
       <c r="V10" s="8"/>
       <c r="W10" s="17"/>
     </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="5">
-        <v>3</v>
-      </c>
+      <c r="D11" s="5"/>
       <c r="H11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="28">
-        <v>43344</v>
-      </c>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
       <c r="N11" s="16"/>
       <c r="O11" s="10" t="s">
         <v>19</v>
@@ -1859,13 +1853,11 @@
       <c r="V11" s="8"/>
       <c r="W11" s="17"/>
     </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="5">
-        <v>4</v>
-      </c>
+      <c r="D12" s="5"/>
       <c r="H12" s="6" t="s">
         <v>8</v>
       </c>
@@ -1889,7 +1881,7 @@
       <c r="V12" s="8"/>
       <c r="W12" s="17"/>
     </row>
-    <row r="13" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H13" s="6" t="s">
         <v>9</v>
       </c>
@@ -1907,7 +1899,7 @@
       <c r="V13" s="11"/>
       <c r="W13" s="19"/>
     </row>
-    <row r="14" spans="2:23" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N14" s="7" t="s">
         <v>29</v>
       </c>
@@ -1915,7 +1907,7 @@
       <c r="V14" s="11"/>
       <c r="W14" s="11"/>
     </row>
-    <row r="15" spans="2:23" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="7" t="s">
         <v>12</v>
       </c>
@@ -1935,11 +1927,11 @@
       <c r="T15" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="U15" s="25"/>
-      <c r="V15" s="25"/>
-      <c r="W15" s="26"/>
-    </row>
-    <row r="16" spans="2:23" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="U15" s="27"/>
+      <c r="V15" s="27"/>
+      <c r="W15" s="28"/>
+    </row>
+    <row r="16" spans="2:23" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B16" s="21" t="s">
         <v>16</v>
       </c>
@@ -1953,9 +1945,9 @@
       <c r="H16" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="26"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="28"/>
       <c r="N16" s="22" t="s">
         <v>17</v>
       </c>
@@ -1973,7 +1965,7 @@
       <c r="V16" s="23"/>
       <c r="W16" s="24"/>
     </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B17" s="22" t="s">
         <v>17</v>
       </c>
@@ -2003,7 +1995,7 @@
       <c r="V17" s="23"/>
       <c r="W17" s="24"/>
     </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B18" s="16"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -2029,7 +2021,7 @@
       <c r="V18" s="8"/>
       <c r="W18" s="17"/>
     </row>
-    <row r="19" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B19" s="16"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -2059,7 +2051,7 @@
       <c r="V19" s="8"/>
       <c r="W19" s="17"/>
     </row>
-    <row r="20" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B20" s="16"/>
       <c r="C20" s="10" t="s">
         <v>18</v>
@@ -2093,7 +2085,7 @@
       <c r="V20" s="8"/>
       <c r="W20" s="17"/>
     </row>
-    <row r="21" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B21" s="16"/>
       <c r="C21" s="10" t="s">
         <v>19</v>
@@ -2127,7 +2119,7 @@
       <c r="V21" s="8"/>
       <c r="W21" s="17"/>
     </row>
-    <row r="22" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="16"/>
       <c r="C22" s="10" t="s">
         <v>20</v>
@@ -2155,7 +2147,7 @@
       <c r="V22" s="11"/>
       <c r="W22" s="19"/>
     </row>
-    <row r="23" spans="2:23" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="18"/>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
@@ -2173,7 +2165,7 @@
       <c r="V23" s="11"/>
       <c r="W23" s="11"/>
     </row>
-    <row r="24" spans="2:23" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="7" t="s">
         <v>26</v>
       </c>
@@ -2193,11 +2185,11 @@
       <c r="T24" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="U24" s="25"/>
-      <c r="V24" s="25"/>
-      <c r="W24" s="26"/>
-    </row>
-    <row r="25" spans="2:23" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="U24" s="27"/>
+      <c r="V24" s="27"/>
+      <c r="W24" s="28"/>
+    </row>
+    <row r="25" spans="2:23" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B25" s="21" t="s">
         <v>16</v>
       </c>
@@ -2211,9 +2203,9 @@
       <c r="H25" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="26"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="28"/>
       <c r="N25" s="22" t="s">
         <v>17</v>
       </c>
@@ -2231,7 +2223,7 @@
       <c r="V25" s="23"/>
       <c r="W25" s="24"/>
     </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B26" s="22" t="s">
         <v>17</v>
       </c>
@@ -2261,7 +2253,7 @@
       <c r="V26" s="23"/>
       <c r="W26" s="24"/>
     </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B27" s="16"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
@@ -2287,7 +2279,7 @@
       <c r="V27" s="8"/>
       <c r="W27" s="17"/>
     </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B28" s="16"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
@@ -2317,7 +2309,7 @@
       <c r="V28" s="8"/>
       <c r="W28" s="17"/>
     </row>
-    <row r="29" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B29" s="16"/>
       <c r="C29" s="10" t="s">
         <v>18</v>
@@ -2351,7 +2343,7 @@
       <c r="V29" s="8"/>
       <c r="W29" s="17"/>
     </row>
-    <row r="30" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B30" s="16"/>
       <c r="C30" s="10" t="s">
         <v>19</v>
@@ -2385,7 +2377,7 @@
       <c r="V30" s="8"/>
       <c r="W30" s="17"/>
     </row>
-    <row r="31" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="16"/>
       <c r="C31" s="10" t="s">
         <v>20</v>
@@ -2413,7 +2405,7 @@
       <c r="V31" s="11"/>
       <c r="W31" s="19"/>
     </row>
-    <row r="32" spans="2:23" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="18"/>
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
@@ -2425,7 +2417,7 @@
       <c r="J32" s="11"/>
       <c r="K32" s="19"/>
     </row>
-    <row r="33" spans="2:23" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="7" t="s">
         <v>27</v>
       </c>
@@ -2436,7 +2428,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="2:23" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:23" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B34" s="21" t="s">
         <v>16</v>
       </c>
@@ -2450,9 +2442,9 @@
       <c r="H34" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="26"/>
+      <c r="I34" s="27"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="28"/>
       <c r="N34" s="12"/>
       <c r="O34" s="13"/>
       <c r="P34" s="13"/>
@@ -2464,7 +2456,7 @@
       <c r="V34" s="13"/>
       <c r="W34" s="15"/>
     </row>
-    <row r="35" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B35" s="22" t="s">
         <v>17</v>
       </c>
@@ -2492,7 +2484,7 @@
       <c r="V35" s="8"/>
       <c r="W35" s="17"/>
     </row>
-    <row r="36" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B36" s="16"/>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
@@ -2516,7 +2508,7 @@
       <c r="V36" s="8"/>
       <c r="W36" s="17"/>
     </row>
-    <row r="37" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B37" s="16"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
@@ -2540,7 +2532,7 @@
       <c r="V37" s="8"/>
       <c r="W37" s="17"/>
     </row>
-    <row r="38" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B38" s="16"/>
       <c r="C38" s="10" t="s">
         <v>18</v>
@@ -2568,7 +2560,7 @@
       <c r="V38" s="8"/>
       <c r="W38" s="17"/>
     </row>
-    <row r="39" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B39" s="16"/>
       <c r="C39" s="10" t="s">
         <v>19</v>
@@ -2596,7 +2588,7 @@
       <c r="V39" s="8"/>
       <c r="W39" s="17"/>
     </row>
-    <row r="40" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B40" s="16"/>
       <c r="C40" s="10" t="s">
         <v>20</v>
@@ -2624,7 +2616,7 @@
       <c r="V40" s="8"/>
       <c r="W40" s="17"/>
     </row>
-    <row r="41" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B41" s="18"/>
       <c r="C41" s="11"/>
       <c r="D41" s="11"/>
@@ -2646,15 +2638,9 @@
       <c r="V41" s="11"/>
       <c r="W41" s="19"/>
     </row>
-    <row r="42" spans="2:23" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="42" spans="2:23" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="I16:K16"/>
     <mergeCell ref="U26:W26"/>
     <mergeCell ref="I35:K35"/>
     <mergeCell ref="I36:K36"/>
@@ -2671,6 +2657,12 @@
     <mergeCell ref="I27:K27"/>
     <mergeCell ref="I25:K25"/>
     <mergeCell ref="I34:K34"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="I16:K16"/>
   </mergeCells>
   <pageMargins left="0.40625" right="0.29166666666666669" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2688,7 +2680,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2700,7 +2692,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>